<commit_message>
Imagens de ficha2 e ficha3 contornos em ficheiro raizes excel
</commit_message>
<xml_diff>
--- a/ANum/Formulas Excel/Raizes.xlsx
+++ b/ANum/Formulas Excel/Raizes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\GitHub\2UFP\ANum\Formulas Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B1A80-772C-4428-A59D-00066745CDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA9D392-409E-4B8F-9C76-B98C4090CC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bissecção" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +121,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -147,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,13 +167,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,13 +526,13 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -577,7 +589,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -611,7 +623,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="4">A3+1</f>
         <v>3</v>
@@ -645,7 +657,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -679,7 +691,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -713,7 +725,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -747,7 +759,7 @@
         <v>1.5625E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -781,7 +793,7 @@
         <v>7.8125E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -815,7 +827,7 @@
         <v>3.90625E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -849,7 +861,7 @@
         <v>1.953125E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -884,7 +896,7 @@
         <v>3.4482758620689689E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>A13+1</f>
         <v>2</v>
@@ -922,7 +934,7 @@
         <v>1.7543859649122823E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" ref="A15:A21" si="17">A14+1</f>
         <v>3</v>
@@ -960,7 +972,7 @@
         <v>8.6956521739130904E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="17"/>
         <v>4</v>
@@ -998,7 +1010,7 @@
         <v>4.366812227074298E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="17"/>
         <v>5</v>
@@ -1036,7 +1048,7 @@
         <v>2.1881838074398561E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="17"/>
         <v>6</v>
@@ -1074,7 +1086,7 @@
         <v>1.0928961748634036E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="17"/>
         <v>7</v>
@@ -1112,7 +1124,7 @@
         <v>5.4614964500269969E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="17"/>
         <v>8</v>
@@ -1150,7 +1162,7 @@
         <v>2.731494127287471E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="17"/>
         <v>9</v>
@@ -1202,9 +1214,9 @@
       <selection pane="bottomLeft" activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1227,7 +1239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1255,7 +1267,7 @@
         <v>0.89451816476754908</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>IF(D2*E2&lt;0,A2,B2)</f>
         <v>1.1054818352324509</v>
@@ -1285,7 +1297,7 @@
         <v>0.8285274244208527</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="3">IF(D3*E3&lt;0,A3,B3)</f>
         <v>1.1714725755791473</v>
@@ -1315,7 +1327,7 @@
         <v>0.79009688027503189</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>1.2099031197249681</v>
@@ -1345,7 +1357,7 @@
         <v>0.76865407232906069</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>1.2313459276709393</v>
@@ -1375,7 +1387,7 @@
         <v>0.75697666139338726</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>1.2430233386066127</v>
@@ -1405,7 +1417,7 @@
         <v>0.75070161140286884</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>1.2492983885971312</v>
@@ -1435,7 +1447,7 @@
         <v>0.74735382477862777</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>1.2526461752213722</v>
@@ -1465,7 +1477,7 @@
         <v>0.74557462931257024</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>1.2544253706874298</v>
@@ -1504,46 +1516,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="7" max="7" width="16.44140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" style="1"/>
     <col min="10" max="10" width="5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="39.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1572,35 +1584,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="4"/>
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="8">
         <v>1</v>
       </c>
       <c r="G4" s="4"/>
       <c r="J4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="8">
         <v>1</v>
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>A4+1</f>
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <f>LN(2*B4+1)</f>
         <v>1.6094379124341003</v>
       </c>
@@ -1612,7 +1624,7 @@
         <f>E4+1</f>
         <v>1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="9">
         <f>F4-((EXP(-F4)-F4^2)/(-EXP(-F4)-2*F4))</f>
         <v>0.73304360524544543</v>
       </c>
@@ -1624,7 +1636,7 @@
         <f>J4+1</f>
         <v>1</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="9">
         <f>0.8</f>
         <v>0.8</v>
       </c>
@@ -1633,7 +1645,7 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A12" si="0">A5+1</f>
         <v>2</v>
@@ -1647,11 +1659,11 @@
         <v>-0.16986921208621442</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ref="E6:E11" si="3">E5+1</f>
+        <f t="shared" ref="E6:E8" si="3">E5+1</f>
         <v>2</v>
       </c>
-      <c r="F6" s="6">
-        <f t="shared" ref="F6:F17" si="4">F5-((EXP(-F5)-F5^2)/(-EXP(-F5)-2*F5))</f>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F8" si="4">F5-((EXP(-F5)-F5^2)/(-EXP(-F5)-2*F5))</f>
         <v>0.70380778632413299</v>
       </c>
       <c r="G6" s="1">
@@ -1662,16 +1674,16 @@
         <f t="shared" ref="J6:J8" si="6">J5+1</f>
         <v>2</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="9">
         <f>K4-((EXP(-K4)-K4^2)*(K5-K4)/(EXP(-K5)-K5^2)-(EXP(-K4)-K4^2))</f>
         <v>1.0309277703546695</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" ref="L6:L25" si="7">K5-K6</f>
+        <f t="shared" ref="L6:L16" si="7">K5-K6</f>
         <v>-0.23092777035466949</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1688,7 +1700,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f t="shared" si="4"/>
         <v>0.70346746833179752</v>
       </c>
@@ -1700,8 +1712,8 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="K7" s="6">
-        <f t="shared" ref="K7:K25" si="8">K5-((EXP(-K5)-K5^2)*(K6-K5)/(EXP(-K6)-K6^2)-(EXP(-K5)-K5^2))</f>
+      <c r="K7" s="5">
+        <f t="shared" ref="K7:K16" si="8">K5-((EXP(-K5)-K5^2)*(K6-K5)/(EXP(-K6)-K6^2)-(EXP(-K5)-K5^2))</f>
         <v>0.54697379976040472</v>
       </c>
       <c r="L7" s="1">
@@ -1709,7 +1721,7 @@
         <v>0.48395397059426482</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1726,7 +1738,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" si="4"/>
         <v>0.70346742249839245</v>
       </c>
@@ -1738,7 +1750,7 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <f t="shared" si="8"/>
         <v>-0.8978033844019</v>
       </c>
@@ -1747,7 +1759,7 @@
         <v>1.4447771841623047</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1760,11 +1772,11 @@
         <f t="shared" si="2"/>
         <v>-2.4135850500302647E-2</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="5"/>
       <c r="J9" s="1">
         <v>5</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <f t="shared" si="8"/>
         <v>1.0715181514511392</v>
       </c>
@@ -1773,7 +1785,7 @@
         <v>-1.9693215358530392</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1786,11 +1798,11 @@
         <f t="shared" si="2"/>
         <v>-1.3414266393589669E-2</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="J10" s="1">
         <v>6</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <f t="shared" si="8"/>
         <v>4.7790188458790333</v>
       </c>
@@ -1799,7 +1811,7 @@
         <v>-3.7075006944278943</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1812,11 +1824,11 @@
         <f t="shared" si="2"/>
         <v>-7.533942846171815E-3</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="5"/>
       <c r="J11" s="1">
         <v>7</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <f t="shared" si="8"/>
         <v>0.13502226637215164</v>
       </c>
@@ -1825,7 +1837,7 @@
         <v>4.6439965795068812</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1838,11 +1850,11 @@
         <f t="shared" si="2"/>
         <v>-4.2563628836007616E-3</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="5"/>
       <c r="J12" s="1">
         <v>8</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <f t="shared" si="8"/>
         <v>-141.99033496913259</v>
       </c>
@@ -1851,7 +1863,7 @@
         <v>142.12535723550474</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" ref="A13:A21" si="9">A12+1</f>
         <v>9</v>
@@ -1864,11 +1876,11 @@
         <f t="shared" si="2"/>
         <v>-2.4127002248959251E-3</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="5"/>
       <c r="J13" s="1">
         <v>9</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <f t="shared" si="8"/>
         <v>0.9904877113768582</v>
       </c>
@@ -1877,7 +1889,7 @@
         <v>-142.98082268050945</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="9"/>
         <v>10</v>
@@ -1890,11 +1902,11 @@
         <f t="shared" si="2"/>
         <v>-1.3702177955308148E-3</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="5"/>
       <c r="J14" s="1">
         <v>10</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <f t="shared" si="8"/>
         <v>1.0905599438786764E+64</v>
       </c>
@@ -1903,7 +1915,7 @@
         <v>-1.0905599438786764E+64</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="9"/>
         <v>11</v>
@@ -1916,11 +1928,11 @@
         <f t="shared" si="2"/>
         <v>-7.7900915958206696E-4</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="5"/>
       <c r="J15" s="1">
         <v>11</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <f t="shared" si="8"/>
         <v>0.38081731801562668</v>
       </c>
@@ -1929,7 +1941,7 @@
         <v>1.0905599438786764E+64</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="9"/>
         <v>12</v>
@@ -1942,11 +1954,11 @@
         <f t="shared" si="2"/>
         <v>-4.4316037670899533E-4</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="5"/>
       <c r="J16" s="1">
         <v>12</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <f t="shared" si="8"/>
         <v>-2.4095707133073647E+192</v>
       </c>
@@ -1955,7 +1967,7 @@
         <v>2.4095707133073647E+192</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="9"/>
         <v>13</v>
@@ -1968,10 +1980,10 @@
         <f t="shared" si="2"/>
         <v>-2.5219140299403975E-4</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="9"/>
         <v>14</v>
@@ -1984,9 +1996,9 @@
         <f t="shared" si="2"/>
         <v>-1.4354417257811392E-4</v>
       </c>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="9"/>
         <v>15</v>
@@ -1999,9 +2011,9 @@
         <f t="shared" si="2"/>
         <v>-8.171273913593069E-5</v>
       </c>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="9"/>
         <v>16</v>
@@ -2014,9 +2026,9 @@
         <f t="shared" si="2"/>
         <v>-4.6518083799185206E-5</v>
       </c>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="9"/>
         <v>17</v>
@@ -2029,9 +2041,9 @@
         <f t="shared" si="2"/>
         <v>-2.648315464237605E-5</v>
       </c>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" ref="A22:A63" si="11">A21+1</f>
         <v>18</v>
@@ -2044,9 +2056,9 @@
         <f t="shared" si="2"/>
         <v>-1.5077406399832682E-5</v>
       </c>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="11"/>
         <v>19</v>
@@ -2059,9 +2071,9 @@
         <f t="shared" si="2"/>
         <v>-8.5839801293730034E-6</v>
       </c>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="11"/>
         <v>20</v>
@@ -2074,9 +2086,9 @@
         <f t="shared" si="2"/>
         <v>-4.8871277471551622E-6</v>
       </c>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="11"/>
         <v>21</v>
@@ -2089,9 +2101,9 @@
         <f t="shared" si="2"/>
         <v>-2.7824049968483422E-6</v>
       </c>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="11"/>
         <v>22</v>
@@ -2105,7 +2117,7 @@
         <v>-1.5841195217802806E-6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="11"/>
         <v>23</v>
@@ -2119,7 +2131,7 @@
         <v>-9.0189522428119062E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="11"/>
         <v>24</v>
@@ -2133,7 +2145,7 @@
         <v>-5.1348118623728567E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -2147,7 +2159,7 @@
         <v>-2.9234330956029453E-7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -2161,7 +2173,7 @@
         <v>-1.6644160005796493E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -2175,7 +2187,7 @@
         <v>-9.4761224200823335E-8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -2189,7 +2201,7 @@
         <v>-5.395099700322703E-8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -2203,7 +2215,7 @@
         <v>-3.0716257981566741E-8</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -2217,7 +2229,7 @@
         <v>-1.7487879144795215E-8</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -2231,7 +2243,7 @@
         <v>-9.9564838595966876E-9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -2245,7 +2257,7 @@
         <v>-5.6685873772721607E-9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f t="shared" si="11"/>
         <v>33</v>
@@ -2259,7 +2271,7 @@
         <v>-3.2273324013232241E-9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f t="shared" si="11"/>
         <v>34</v>
@@ -2273,7 +2285,7 @@
         <v>-1.8374373134122379E-9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f t="shared" si="11"/>
         <v>35</v>
@@ -2287,7 +2299,7 @@
         <v>-1.0461198574063246E-9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f t="shared" si="11"/>
         <v>36</v>
@@ -2301,7 +2313,7 @@
         <v>-5.9559379650409028E-10</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f t="shared" si="11"/>
         <v>37</v>
@@ -2315,7 +2327,7 @@
         <v>-3.3909319796521231E-10</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f t="shared" si="11"/>
         <v>38</v>
@@ -2329,7 +2341,7 @@
         <v>-1.9305801401969802E-10</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f t="shared" si="11"/>
         <v>39</v>
@@ -2343,7 +2355,7 @@
         <v>-1.0991496601775452E-10</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f t="shared" si="11"/>
         <v>40</v>
@@ -2357,7 +2369,7 @@
         <v>-6.2578608961416649E-11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f t="shared" si="11"/>
         <v>41</v>
@@ -2371,7 +2383,7 @@
         <v>-3.5628389127850824E-11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f t="shared" si="11"/>
         <v>42</v>
@@ -2385,7 +2397,7 @@
         <v>-2.0284440793716385E-11</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <f t="shared" si="11"/>
         <v>43</v>
@@ -2399,7 +2411,7 @@
         <v>-1.1548761946755803E-11</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f t="shared" si="11"/>
         <v>44</v>
@@ -2413,7 +2425,7 @@
         <v>-6.5749627964351021E-12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f t="shared" si="11"/>
         <v>45</v>
@@ -2427,7 +2439,7 @@
         <v>-3.7434499944311028E-12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f t="shared" si="11"/>
         <v>46</v>
@@ -2441,7 +2453,7 @@
         <v>-2.1311841180704505E-12</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f t="shared" si="11"/>
         <v>47</v>
@@ -2455,7 +2467,7 @@
         <v>-1.2134737659152961E-12</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f t="shared" si="11"/>
         <v>48</v>
@@ -2469,7 +2481,7 @@
         <v>-6.907807659217724E-13</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f t="shared" si="11"/>
         <v>49</v>
@@ -2483,7 +2495,7 @@
         <v>-3.9324099532223045E-13</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f t="shared" si="11"/>
         <v>50</v>
@@ -2497,7 +2509,7 @@
         <v>-2.2404300636935659E-13</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f t="shared" si="11"/>
         <v>51</v>
@@ -2511,7 +2523,7 @@
         <v>-1.2745360322696797E-13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f t="shared" si="11"/>
         <v>52</v>
@@ -2525,7 +2537,7 @@
         <v>-7.2608585810485238E-14</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f t="shared" si="11"/>
         <v>53</v>
@@ -2539,7 +2551,7 @@
         <v>-4.1300296516055823E-14</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f t="shared" si="11"/>
         <v>54</v>
@@ -2553,7 +2565,7 @@
         <v>-2.3536728122053319E-14</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f t="shared" si="11"/>
         <v>55</v>
@@ -2567,7 +2579,7 @@
         <v>-1.3322676295501878E-14</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f t="shared" si="11"/>
         <v>56</v>
@@ -2581,7 +2593,7 @@
         <v>-7.7715611723760958E-15</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f t="shared" si="11"/>
         <v>57</v>
@@ -2595,7 +2607,7 @@
         <v>-4.4408920985006262E-15</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <f t="shared" si="11"/>
         <v>58</v>
@@ -2609,7 +2621,7 @@
         <v>-2.4424906541753444E-15</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f t="shared" si="11"/>
         <v>59</v>

</xml_diff>